<commit_message>
Päivitetty Livin beaconien major-numerot ja lisätty kenttä josta näkyy numerot desimaalilukuna
</commit_message>
<xml_diff>
--- a/Beaconit.xlsx
+++ b/Beaconit.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miko.thusberg/OneDrive - Gofore Oy/Cases/Livi/Beaconit/Livi pilotti/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smartpirtti/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5660" yWindow="460" windowWidth="23140" windowHeight="16120" tabRatio="500"/>
+    <workbookView xWindow="3380" yWindow="9940" windowWidth="20420" windowHeight="16120" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Livi" sheetId="1" r:id="rId1"/>
@@ -193,7 +193,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="109">
   <si>
     <t>Beaconit</t>
   </si>
@@ -514,6 +514,12 @@
   </si>
   <si>
     <t>Koodi puuttuu</t>
+  </si>
+  <si>
+    <t>FF44</t>
+  </si>
+  <si>
+    <t>Dec</t>
   </si>
 </sst>
 </file>
@@ -599,14 +605,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -634,13 +664,40 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="5">
-    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="29">
+    <cellStyle name="Avattu hyperlinkki" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="1" builtinId="8"/>
+    <cellStyle name="Norm." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -918,10 +975,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I195"/>
+  <dimension ref="A1:J195"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D139" sqref="D139"/>
+    <sheetView topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -929,19 +986,20 @@
     <col min="1" max="1" width="12.33203125" customWidth="1"/>
     <col min="2" max="2" width="21" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.6640625" style="8" customWidth="1"/>
-    <col min="5" max="5" width="30.6640625" customWidth="1"/>
-    <col min="6" max="6" width="21.1640625" style="1" customWidth="1"/>
-    <col min="7" max="8" width="9.1640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="15" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" customWidth="1"/>
+    <col min="7" max="7" width="21.1640625" style="1" customWidth="1"/>
+    <col min="8" max="9" width="9.1640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -949,30 +1007,31 @@
       <c r="C3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="16"/>
+      <c r="E3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
@@ -980,7 +1039,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>28</v>
       </c>
@@ -988,7 +1047,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>25</v>
       </c>
@@ -996,7 +1055,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>26</v>
       </c>
@@ -1004,18 +1063,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="s">
         <v>83</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>14</v>
       </c>
@@ -1023,34 +1082,34 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="11"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E13" s="11"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="11"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D15" s="10"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E14" s="11"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E15" s="10"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="10"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E16" s="10"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>11</v>
       </c>
@@ -1058,7 +1117,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>28</v>
       </c>
@@ -1066,7 +1125,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>25</v>
       </c>
@@ -1074,7 +1133,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>26</v>
       </c>
@@ -1082,7 +1141,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>1</v>
       </c>
@@ -1090,23 +1149,31 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D22" s="15">
+        <f>HEX2DEC(C22)</f>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D23" s="15">
+        <f>HEX2DEC(C23)</f>
+        <v>2089</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>14</v>
       </c>
@@ -1114,7 +1181,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>28</v>
       </c>
@@ -1122,7 +1189,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>25</v>
       </c>
@@ -1130,7 +1197,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
         <v>26</v>
       </c>
@@ -1138,7 +1205,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>1</v>
       </c>
@@ -1146,35 +1213,43 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+      <c r="D30" s="15">
+        <f>HEX2DEC(C30)</f>
+        <v>65348</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="D31" s="15">
+        <f>HEX2DEC(C31)</f>
+        <v>2089</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="H31" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="I31" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="I31" s="1" t="s">
+      <c r="J31" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>9</v>
       </c>
@@ -1182,30 +1257,33 @@
       <c r="C33" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="9" t="s">
+      <c r="D33" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="E33" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="F33" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B36" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
         <v>11</v>
       </c>
@@ -1213,7 +1291,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
         <v>28</v>
       </c>
@@ -1221,7 +1299,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
         <v>25</v>
       </c>
@@ -1229,7 +1307,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
         <v>26</v>
       </c>
@@ -1237,18 +1315,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C41" t="s">
         <v>79</v>
       </c>
-      <c r="D41" s="10" t="s">
+      <c r="E41" s="10" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
         <v>14</v>
       </c>
@@ -1256,7 +1334,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
         <v>28</v>
       </c>
@@ -1264,7 +1342,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
         <v>25</v>
       </c>
@@ -1272,7 +1350,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
         <v>26</v>
       </c>
@@ -1280,45 +1358,45 @@
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C46" t="s">
         <v>81</v>
       </c>
-      <c r="D46" s="10" t="s">
+      <c r="E46" s="10" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D47" s="11"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E47" s="11"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D48" s="11"/>
-    </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D49" s="10"/>
-    </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E48" s="11"/>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="E49" s="10"/>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B50" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D50" s="10"/>
-    </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E50" s="10"/>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B51" s="1" t="s">
         <v>11</v>
       </c>
@@ -1326,7 +1404,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B52" s="1" t="s">
         <v>28</v>
       </c>
@@ -1334,7 +1412,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B53" s="1" t="s">
         <v>25</v>
       </c>
@@ -1342,7 +1420,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B54" s="1" t="s">
         <v>26</v>
       </c>
@@ -1350,7 +1428,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B55" s="1" t="s">
         <v>1</v>
       </c>
@@ -1358,35 +1436,43 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B56" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D56" s="15">
+        <f>HEX2DEC(C56)</f>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B57" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F57" s="1" t="s">
+      <c r="D57" s="15">
+        <f>HEX2DEC(C57)</f>
+        <v>4138</v>
+      </c>
+      <c r="G57" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="G57" s="1" t="s">
+      <c r="H57" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H57" s="1" t="s">
+      <c r="I57" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="I57" s="1" t="s">
+      <c r="J57" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B59" s="1" t="s">
         <v>14</v>
       </c>
@@ -1394,7 +1480,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B60" s="1" t="s">
         <v>28</v>
       </c>
@@ -1402,7 +1488,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B61" s="1" t="s">
         <v>25</v>
       </c>
@@ -1410,7 +1496,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B62" s="1" t="s">
         <v>26</v>
       </c>
@@ -1418,7 +1504,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B63" s="1" t="s">
         <v>1</v>
       </c>
@@ -1426,23 +1512,31 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B64" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+      <c r="D64" s="15">
+        <f>HEX2DEC(C64)</f>
+        <v>65348</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B65" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D65" s="15">
+        <f>HEX2DEC(C65)</f>
+        <v>4138</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
         <v>33</v>
       </c>
@@ -1450,30 +1544,31 @@
       <c r="C67" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D67" s="9" t="s">
+      <c r="D67" s="16"/>
+      <c r="E67" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E67" s="4" t="s">
+      <c r="F67" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B68" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E68" t="s">
+      <c r="F68" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B70" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B71" s="1" t="s">
         <v>11</v>
       </c>
@@ -1481,7 +1576,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B72" s="1" t="s">
         <v>28</v>
       </c>
@@ -1489,7 +1584,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B73" s="1" t="s">
         <v>25</v>
       </c>
@@ -1497,7 +1592,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B74" s="1" t="s">
         <v>26</v>
       </c>
@@ -1505,18 +1600,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="B75" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C75" t="s">
         <v>79</v>
       </c>
-      <c r="D75" s="10" t="s">
+      <c r="E75" s="10" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B76" s="1" t="s">
         <v>14</v>
       </c>
@@ -1524,7 +1619,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B77" s="1" t="s">
         <v>28</v>
       </c>
@@ -1532,7 +1627,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B78" s="1" t="s">
         <v>25</v>
       </c>
@@ -1540,7 +1635,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B79" s="1" t="s">
         <v>26</v>
       </c>
@@ -1548,45 +1643,45 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="B80" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C80" t="s">
         <v>81</v>
       </c>
-      <c r="D80" s="10" t="s">
+      <c r="E80" s="10" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B81" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D81" s="11"/>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E81" s="11"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B82" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D82" s="11"/>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D83" s="10"/>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E82" s="11"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E83" s="10"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B84" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D84" s="10"/>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E84" s="10"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B85" s="1" t="s">
         <v>11</v>
       </c>
@@ -1594,7 +1689,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B86" s="1" t="s">
         <v>28</v>
       </c>
@@ -1602,7 +1697,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B87" s="1" t="s">
         <v>25</v>
       </c>
@@ -1610,7 +1705,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B88" s="1" t="s">
         <v>26</v>
       </c>
@@ -1618,7 +1713,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B89" s="1" t="s">
         <v>1</v>
       </c>
@@ -1626,35 +1721,43 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B90" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D90" s="15">
+        <f>HEX2DEC(C90)</f>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B91" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F91" s="1" t="s">
+      <c r="D91" s="15">
+        <f>HEX2DEC(C91)</f>
+        <v>4137</v>
+      </c>
+      <c r="G91" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="G91" s="1" t="s">
+      <c r="H91" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H91" s="1" t="s">
+      <c r="I91" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="I91" s="1" t="s">
+      <c r="J91" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B93" s="1" t="s">
         <v>14</v>
       </c>
@@ -1662,7 +1765,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" s="6" t="s">
         <v>35</v>
       </c>
@@ -1670,30 +1773,31 @@
       <c r="C95" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D95" s="9" t="s">
+      <c r="D95" s="16"/>
+      <c r="E95" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E95" s="4" t="s">
+      <c r="F95" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B96" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E96" t="s">
+      <c r="F96" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B98" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B99" s="1" t="s">
         <v>11</v>
       </c>
@@ -1701,7 +1805,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B100" s="1" t="s">
         <v>28</v>
       </c>
@@ -1709,7 +1813,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B101" s="1" t="s">
         <v>25</v>
       </c>
@@ -1717,7 +1821,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B102" s="1" t="s">
         <v>26</v>
       </c>
@@ -1725,18 +1829,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="103" spans="2:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:5" ht="32" x14ac:dyDescent="0.2">
       <c r="B103" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C103" t="s">
         <v>83</v>
       </c>
-      <c r="D103" s="10" t="s">
+      <c r="E103" s="10" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B104" s="1" t="s">
         <v>14</v>
       </c>
@@ -1744,34 +1848,34 @@
         <v>17</v>
       </c>
     </row>
-    <row r="105" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B105" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D105" s="11"/>
-    </row>
-    <row r="106" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E105" s="11"/>
+    </row>
+    <row r="106" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B106" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D106" s="11"/>
-    </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D107" s="10"/>
-    </row>
-    <row r="108" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E106" s="11"/>
+    </row>
+    <row r="107" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E107" s="10"/>
+    </row>
+    <row r="108" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B108" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D108" s="10"/>
-    </row>
-    <row r="109" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E108" s="10"/>
+    </row>
+    <row r="109" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B109" s="1" t="s">
         <v>11</v>
       </c>
@@ -1779,7 +1883,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="110" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B110" s="1" t="s">
         <v>28</v>
       </c>
@@ -1787,7 +1891,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="111" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B111" s="1" t="s">
         <v>25</v>
       </c>
@@ -1795,7 +1899,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="112" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B112" s="1" t="s">
         <v>26</v>
       </c>
@@ -1803,7 +1907,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B113" s="1" t="s">
         <v>1</v>
       </c>
@@ -1811,35 +1915,43 @@
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B114" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D114" s="15">
+        <f>HEX2DEC(C114)</f>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B115" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F115" s="1" t="s">
+      <c r="D115" s="15">
+        <f>HEX2DEC(C115)</f>
+        <v>8233</v>
+      </c>
+      <c r="G115" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="G115" s="1" t="s">
+      <c r="H115" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="H115" s="1" t="s">
+      <c r="I115" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="I115" s="14" t="s">
+      <c r="J115" s="14" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B117" s="1" t="s">
         <v>14</v>
       </c>
@@ -1847,7 +1959,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A119" s="6" t="s">
         <v>37</v>
       </c>
@@ -1855,30 +1967,31 @@
       <c r="C119" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D119" s="9" t="s">
+      <c r="D119" s="16"/>
+      <c r="E119" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E119" s="4" t="s">
+      <c r="F119" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B120" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E120" t="s">
+      <c r="F120" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B122" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B123" s="1" t="s">
         <v>11</v>
       </c>
@@ -1886,7 +1999,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B124" s="1" t="s">
         <v>28</v>
       </c>
@@ -1894,7 +2007,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B125" s="1" t="s">
         <v>25</v>
       </c>
@@ -1902,7 +2015,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B126" s="1" t="s">
         <v>26</v>
       </c>
@@ -1910,18 +2023,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="127" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="B127" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C127" t="s">
         <v>83</v>
       </c>
-      <c r="D127" s="10" t="s">
+      <c r="E127" s="10" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B128" s="1" t="s">
         <v>14</v>
       </c>
@@ -1929,34 +2042,34 @@
         <v>17</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B129" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D129" s="11"/>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E129" s="11"/>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B130" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D130" s="11"/>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D131" s="10"/>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E130" s="11"/>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E131" s="10"/>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B132" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D132" s="10"/>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E132" s="10"/>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B133" s="1" t="s">
         <v>11</v>
       </c>
@@ -1964,7 +2077,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B134" s="1" t="s">
         <v>28</v>
       </c>
@@ -1972,7 +2085,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B135" s="1" t="s">
         <v>25</v>
       </c>
@@ -1980,7 +2093,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B136" s="1" t="s">
         <v>26</v>
       </c>
@@ -1988,7 +2101,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B137" s="1" t="s">
         <v>1</v>
       </c>
@@ -1996,35 +2109,43 @@
         <v>2</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B138" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D138" s="15">
+        <f>HEX2DEC(C138)</f>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B139" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="F139" s="1" t="s">
+      <c r="D139" s="15">
+        <f>HEX2DEC(C139)</f>
+        <v>8234</v>
+      </c>
+      <c r="G139" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="G139" s="1" t="s">
+      <c r="H139" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="H139" s="1" t="s">
+      <c r="I139" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="I139" s="1" t="s">
+      <c r="J139" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B141" s="1" t="s">
         <v>14</v>
       </c>
@@ -2032,7 +2153,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A143" s="6" t="s">
         <v>39</v>
       </c>
@@ -2040,30 +2161,31 @@
       <c r="C143" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D143" s="9" t="s">
+      <c r="D143" s="16"/>
+      <c r="E143" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E143" s="4" t="s">
+      <c r="F143" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B144" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E144" t="s">
+      <c r="F144" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="146" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="146" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B146" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="147" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="147" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B147" s="1" t="s">
         <v>11</v>
       </c>
@@ -2071,29 +2193,30 @@
         <v>17</v>
       </c>
     </row>
-    <row r="148" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="148" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B148" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="149" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B149" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="150" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B150" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="151" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B151" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C151" s="2"/>
-      <c r="D151" s="10"/>
-    </row>
-    <row r="152" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D151" s="17"/>
+      <c r="E151" s="10"/>
+    </row>
+    <row r="152" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B152" s="1" t="s">
         <v>14</v>
       </c>
@@ -2101,34 +2224,34 @@
         <v>17</v>
       </c>
     </row>
-    <row r="153" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B153" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D153" s="11"/>
-    </row>
-    <row r="154" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E153" s="11"/>
+    </row>
+    <row r="154" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B154" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C154" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D154" s="11"/>
-    </row>
-    <row r="155" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D155" s="10"/>
-    </row>
-    <row r="156" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E154" s="11"/>
+    </row>
+    <row r="155" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E155" s="10"/>
+    </row>
+    <row r="156" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B156" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D156" s="10"/>
-    </row>
-    <row r="157" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E156" s="10"/>
+    </row>
+    <row r="157" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B157" s="1" t="s">
         <v>11</v>
       </c>
@@ -2136,7 +2259,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="158" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B158" s="1" t="s">
         <v>28</v>
       </c>
@@ -2144,7 +2267,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="159" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="159" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B159" s="1" t="s">
         <v>25</v>
       </c>
@@ -2152,7 +2275,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="160" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="160" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B160" s="1" t="s">
         <v>26</v>
       </c>
@@ -2160,7 +2283,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B161" s="1" t="s">
         <v>1</v>
       </c>
@@ -2168,35 +2291,43 @@
         <v>2</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B162" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C162" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D162" s="15">
+        <f>HEX2DEC(C162)</f>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B163" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F163" s="1" t="s">
+      <c r="D163" s="15">
+        <f>HEX2DEC(C163)</f>
+        <v>1066</v>
+      </c>
+      <c r="G163" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="G163" s="1" t="s">
+      <c r="H163" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="H163" s="1" t="s">
+      <c r="I163" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="I163" s="1" t="s">
+      <c r="J163" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B165" s="1" t="s">
         <v>14</v>
       </c>
@@ -2204,7 +2335,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A167" s="6" t="s">
         <v>41</v>
       </c>
@@ -2212,31 +2343,32 @@
       <c r="C167" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D167" s="9" t="s">
+      <c r="D167" s="16"/>
+      <c r="E167" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E167" s="4" t="s">
+      <c r="F167" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B168" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C168" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D168" s="12"/>
-      <c r="E168" t="s">
+      <c r="E168" s="12"/>
+      <c r="F168" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B170" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B171" s="1" t="s">
         <v>11</v>
       </c>
@@ -2244,7 +2376,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B172" s="1" t="s">
         <v>28</v>
       </c>
@@ -2252,7 +2384,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B173" s="1" t="s">
         <v>25</v>
       </c>
@@ -2260,7 +2392,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B174" s="1" t="s">
         <v>26</v>
       </c>
@@ -2268,18 +2400,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="175" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="B175" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C175" t="s">
         <v>101</v>
       </c>
-      <c r="D175" s="10" t="s">
+      <c r="E175" s="10" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B176" s="1" t="s">
         <v>14</v>
       </c>
@@ -2287,34 +2419,34 @@
         <v>17</v>
       </c>
     </row>
-    <row r="177" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="177" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B177" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C177" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D177" s="11"/>
-    </row>
-    <row r="178" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E177" s="11"/>
+    </row>
+    <row r="178" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B178" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C178" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D178" s="11"/>
-    </row>
-    <row r="179" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D179" s="10"/>
-    </row>
-    <row r="180" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E178" s="11"/>
+    </row>
+    <row r="179" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E179" s="10"/>
+    </row>
+    <row r="180" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B180" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D180" s="10"/>
-    </row>
-    <row r="181" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E180" s="10"/>
+    </row>
+    <row r="181" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B181" s="1" t="s">
         <v>11</v>
       </c>
@@ -2322,37 +2454,37 @@
         <v>17</v>
       </c>
     </row>
-    <row r="182" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="182" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B182" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="183" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="183" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B183" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="184" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="184" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B184" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="185" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="185" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B185" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="186" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B186" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="187" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="187" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B187" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="189" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="189" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B189" s="1" t="s">
         <v>14</v>
       </c>
@@ -2360,7 +2492,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="190" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="190" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B190" s="1" t="s">
         <v>28</v>
       </c>
@@ -2368,7 +2500,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="191" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="191" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B191" s="1" t="s">
         <v>25</v>
       </c>
@@ -2376,7 +2508,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="192" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="192" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B192" s="1" t="s">
         <v>26</v>
       </c>
@@ -2384,7 +2516,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="193" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="193" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B193" s="1" t="s">
         <v>1</v>
       </c>
@@ -2392,22 +2524,30 @@
         <v>2</v>
       </c>
     </row>
-    <row r="194" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="194" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B194" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="195" spans="2:4" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+      <c r="D194" s="15">
+        <f>HEX2DEC(C194)</f>
+        <v>65348</v>
+      </c>
+    </row>
+    <row r="195" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B195" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D195" s="8" t="s">
+      <c r="D195" s="15">
+        <f>HEX2DEC(C195)</f>
+        <v>68</v>
+      </c>
+      <c r="E195" s="8" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2422,9 +2562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2458,7 +2596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A33"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>